<commit_message>
Training Deviation Log 출력 / 수료증 출력 / 한글깨짐 해결 / 20201-02-09
</commit_message>
<xml_diff>
--- a/src/main/resources/com/cauh/iso/xdocreport/SOP_Training_Deviation_Log.xlsx
+++ b/src/main/resources/com/cauh/iso/xdocreport/SOP_Training_Deviation_Log.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Quality Management Affairs\QA\07. CAUH_ISO14155\02. ISO-SOP RF Development\CAUH-QM002 v1.0_Overall rule for SOP Management\Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SafeSoft\IdeaProjects\SOP\cauh-iso-ms\src\main\resources\com\cauh\iso\xdocreport\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0060D4D3-DF91-4C5B-B5F5-32CD3CF44A20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9105"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOP TR Deviation Log" sheetId="1" r:id="rId1"/>
@@ -26,6 +27,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>SafeSoft</author>
+  </authors>
+  <commentList>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{C4AC9832-B28B-430C-BE2D-3510190626EE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SafeSoft:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="R6")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
@@ -175,12 +210,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.0_);[Red]\(0.0\)"/>
     <numFmt numFmtId="177" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +357,19 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -944,6 +992,87 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -964,87 +1093,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1086,7 +1134,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
@@ -1121,6 +1175,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1385,152 +1443,152 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="80" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A5" sqref="A5:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
     <col min="2" max="2" width="20.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.75" style="1" customWidth="1"/>
-    <col min="6" max="7" width="14.125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="11.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.19921875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.69921875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="14.09765625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="11.8984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3984375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.69921875" style="1" customWidth="1"/>
     <col min="12" max="12" width="17" style="1" customWidth="1"/>
-    <col min="13" max="13" width="23.75" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="18.375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11.25" style="1" customWidth="1"/>
+    <col min="13" max="13" width="23.69921875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.59765625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.3984375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.19921875" style="1" customWidth="1"/>
     <col min="17" max="17" width="10.5" style="1" customWidth="1"/>
     <col min="18" max="18" width="12.5" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.75" style="1"/>
+    <col min="19" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="24.75" customHeight="1">
-      <c r="A1" s="55"/>
-      <c r="B1" s="56"/>
-      <c r="C1" s="63" t="s">
+      <c r="A1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="64"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="45"/>
     </row>
     <row r="2" spans="1:18" ht="34.5" customHeight="1">
-      <c r="A2" s="57"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="61" t="s">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="62"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="43"/>
     </row>
     <row r="3" spans="1:18" ht="24" customHeight="1" thickBot="1">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="65" t="s">
+      <c r="A3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="66" t="s">
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="66" t="s">
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="67"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="69"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="50"/>
     </row>
-    <row r="4" spans="1:18" ht="17.25" thickBot="1"/>
+    <row r="4" spans="1:18" ht="18" thickBot="1"/>
     <row r="5" spans="1:18" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="38" t="s">
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="38"/>
-      <c r="J5" s="48" t="s">
+      <c r="I5" s="65"/>
+      <c r="J5" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="49"/>
-      <c r="L5" s="53" t="s">
+      <c r="K5" s="56"/>
+      <c r="L5" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="43" t="s">
+      <c r="M5" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="N5" s="50" t="s">
+      <c r="N5" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="O5" s="43" t="s">
+      <c r="O5" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="50" t="s">
+      <c r="P5" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="Q5" s="44" t="s">
+      <c r="Q5" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="46" t="s">
+      <c r="R5" s="53" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:18" s="4" customFormat="1" ht="38.25" customHeight="1" thickBot="1">
-      <c r="A6" s="37"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1558,15 +1616,15 @@
       <c r="K6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="54"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="47"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="52"/>
+      <c r="R6" s="54"/>
     </row>
-    <row r="7" spans="1:18" ht="84.95" customHeight="1">
+    <row r="7" spans="1:18" ht="84.9" customHeight="1">
       <c r="A7" s="20">
         <v>1</v>
       </c>
@@ -1602,7 +1660,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="84.95" customHeight="1">
+    <row r="8" spans="1:18" ht="84.9" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
@@ -1624,7 +1682,7 @@
       </c>
       <c r="R8" s="32"/>
     </row>
-    <row r="9" spans="1:18" ht="84.95" customHeight="1">
+    <row r="9" spans="1:18" ht="84.9" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
@@ -1644,7 +1702,7 @@
       <c r="Q9" s="34"/>
       <c r="R9" s="18"/>
     </row>
-    <row r="10" spans="1:18" ht="84.95" customHeight="1">
+    <row r="10" spans="1:18" ht="84.9" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
@@ -1664,7 +1722,7 @@
       <c r="Q10" s="13"/>
       <c r="R10" s="18"/>
     </row>
-    <row r="11" spans="1:18" ht="84.95" customHeight="1">
+    <row r="11" spans="1:18" ht="84.9" customHeight="1">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
@@ -1686,8 +1744,8 @@
     </row>
     <row r="12" spans="1:18">
       <c r="B12" s="19"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
     </row>
     <row r="14" spans="1:18">
       <c r="B14" s="30" t="s">
@@ -1699,12 +1757,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="C2:R2"/>
-    <mergeCell ref="C1:R1"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="M3:R3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C5:G5"/>
     <mergeCell ref="Q5:Q6"/>
     <mergeCell ref="R5:R6"/>
     <mergeCell ref="J5:K5"/>
@@ -1713,11 +1770,12 @@
     <mergeCell ref="P5:P6"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C2:R2"/>
+    <mergeCell ref="C1:R1"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="M3:R3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -1730,5 +1788,6 @@
 CONFIDENTIAL </oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>